<commit_message>
extended a test & match password function
</commit_message>
<xml_diff>
--- a/test_records.xlsx
+++ b/test_records.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-workspace\HackMe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADD42E3-55A6-478F-844B-43F04E6EEB96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10633231-FC00-4A41-9BEF-42977515B52E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10546" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>testGetPassword()</t>
+  </si>
+  <si>
+    <t>Null pointer exception - send in null as difficulty</t>
+  </si>
+  <si>
+    <t>Fixed, added condition to check for null</t>
   </si>
 </sst>
 </file>
@@ -486,7 +492,7 @@
   <dimension ref="B1:G302"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -494,7 +500,7 @@
     <col min="2" max="2" width="10.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.46484375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
@@ -620,16 +626,32 @@
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B10" s="10"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="B10" s="10">
+        <v>43800</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B11" s="5"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="B11" s="10">
+        <v>43800</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B12" s="5"/>

</xml_diff>

<commit_message>
redesigned structure & implemented some methods
</commit_message>
<xml_diff>
--- a/test_records.xlsx
+++ b/test_records.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-workspace\HackMe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A8CBAA1-4B9F-490A-8E31-2F394CCEAB30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D8B7DE-C6A9-47E8-AD88-AFBC17A2DA6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10546" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="31">
   <si>
     <t>Date</t>
   </si>
@@ -85,6 +85,45 @@
   </si>
   <si>
     <t>Regression tested all others as well, they all passed and so did not include them here</t>
+  </si>
+  <si>
+    <t>only test base created</t>
+  </si>
+  <si>
+    <t>testRestartOnClick()</t>
+  </si>
+  <si>
+    <t>testInitialiseGameWordVariables()</t>
+  </si>
+  <si>
+    <t>testWordOnClick()</t>
+  </si>
+  <si>
+    <t>testStartEndGameScene()</t>
+  </si>
+  <si>
+    <t>testSetDifficulty()</t>
+  </si>
+  <si>
+    <t>testStartGameScene()</t>
+  </si>
+  <si>
+    <t>testSetStage()</t>
+  </si>
+  <si>
+    <t>testStart()</t>
+  </si>
+  <si>
+    <t>testMain()</t>
+  </si>
+  <si>
+    <t>testOnKeyPressed()</t>
+  </si>
+  <si>
+    <t>estCloseOnClick()</t>
+  </si>
+  <si>
+    <t>testSetFinalScore()</t>
   </si>
 </sst>
 </file>
@@ -199,7 +238,49 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE84E18"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE84E18"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE84E18"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -500,14 +581,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5534E86-464A-458A-BDC4-36EF59462518}">
   <dimension ref="B1:G302"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="10.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.46484375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="41.265625" bestFit="1" customWidth="1"/>
   </cols>
@@ -697,76 +778,172 @@
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B14" s="5"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="B14" s="5">
+        <v>43802</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B15" s="5"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="B15" s="5">
+        <v>43802</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B16" s="5"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="B16" s="5">
+        <v>43802</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B17" s="5"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="B17" s="5">
+        <v>43802</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B18" s="5"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="B18" s="5">
+        <v>43802</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B19" s="5"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="B19" s="5">
+        <v>43802</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B20" s="5"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="B20" s="5">
+        <v>43802</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B21" s="5"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
+      <c r="B21" s="5">
+        <v>43802</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B22" s="5"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+      <c r="B22" s="5">
+        <v>43802</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B23" s="5"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
+      <c r="B23" s="5">
+        <v>43802</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B24" s="5"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+      <c r="B24" s="5">
+        <v>43802</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B25" s="5"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+      <c r="B25" s="5">
+        <v>43802</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B26" s="5"/>
@@ -2431,12 +2608,20 @@
       <c r="E302" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:E100">
-    <cfRule type="expression" dxfId="1" priority="3">
+  <conditionalFormatting sqref="B3:E19 B20:B25 B26:E100 D20:E22 D23 B24:D25 E23:E25">
+    <cfRule type="expression" dxfId="3" priority="9">
       <formula>EXACT($D3,$G$3)</formula>
     </cfRule>
+    <cfRule type="expression" dxfId="2" priority="7">
+      <formula>EXACT($D3, $G$4)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20:C23">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>EXACT($D3, $G$4)</formula>
+      <formula>EXACT($D20, $G$4)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>EXACT($D20,$G$3)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">

</xml_diff>

<commit_message>
metrics & tests & show score on end screen
</commit_message>
<xml_diff>
--- a/test_records.xlsx
+++ b/test_records.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-workspace\HackMe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87B4865-1A08-41B7-8DFF-C76B34E8547B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E37F7B-07E5-4208-930A-83707B5E1F9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10546" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="53">
   <si>
     <t>Date</t>
   </si>
@@ -381,21 +381,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE84E18"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill>
@@ -736,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5534E86-464A-458A-BDC4-36EF59462518}">
-  <dimension ref="A1:G320"/>
+  <dimension ref="A1:G318"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -833,7 +819,7 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B7" s="4">
-        <v>43799</v>
+        <v>43797</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>4</v>
@@ -875,7 +861,7 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B10" s="4">
-        <v>43797</v>
+        <v>43799</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>4</v>
@@ -990,18 +976,16 @@
         <v>43801</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B19" s="10">
-        <v>43802</v>
+      <c r="B19" s="5">
+        <v>43801</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>9</v>
@@ -1009,96 +993,82 @@
       <c r="D19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B20" s="10">
-        <v>43802</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="B20" s="5">
+        <v>43801</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B21" s="10">
-        <v>43802</v>
+      <c r="B21" s="5">
+        <v>43801</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B22" s="10">
         <v>43802</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="C22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B23" s="10">
         <v>43802</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B24" s="10">
         <v>43802</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="C24" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="4"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="11">
+      <c r="B25" s="10">
         <v>43802</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="C25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
@@ -1108,7 +1078,7 @@
         <v>43802</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>5</v>
@@ -1125,7 +1095,7 @@
         <v>43802</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D27" s="12" t="s">
         <v>5</v>
@@ -1142,7 +1112,7 @@
         <v>43802</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>5</v>
@@ -1159,7 +1129,7 @@
         <v>43802</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D29" s="12" t="s">
         <v>5</v>
@@ -1176,7 +1146,7 @@
         <v>43802</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>5</v>
@@ -1193,7 +1163,7 @@
         <v>43802</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D31" s="12" t="s">
         <v>5</v>
@@ -1210,7 +1180,7 @@
         <v>43802</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D32" s="12" t="s">
         <v>5</v>
@@ -1227,7 +1197,7 @@
         <v>43802</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D33" s="12" t="s">
         <v>5</v>
@@ -1244,7 +1214,7 @@
         <v>43802</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D34" s="12" t="s">
         <v>5</v>
@@ -1261,7 +1231,7 @@
         <v>43802</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D35" s="12" t="s">
         <v>5</v>
@@ -1278,7 +1248,7 @@
         <v>43802</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D36" s="12" t="s">
         <v>5</v>
@@ -1288,17 +1258,17 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B37" s="5">
-        <v>43804</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>33</v>
+      <c r="B37" s="11">
+        <v>43802</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.45">
@@ -1306,7 +1276,7 @@
         <v>43804</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>5</v>
@@ -1320,7 +1290,7 @@
         <v>43804</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>5</v>
@@ -1334,7 +1304,7 @@
         <v>43804</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>5</v>
@@ -1348,7 +1318,7 @@
         <v>43804</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>5</v>
@@ -1362,7 +1332,7 @@
         <v>43804</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>5</v>
@@ -1376,7 +1346,7 @@
         <v>43804</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>5</v>
@@ -1390,7 +1360,7 @@
         <v>43804</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>5</v>
@@ -1404,7 +1374,7 @@
         <v>43804</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>5</v>
@@ -1418,7 +1388,7 @@
         <v>43804</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>5</v>
@@ -1432,7 +1402,7 @@
         <v>43804</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>5</v>
@@ -1443,16 +1413,16 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B48" s="5">
-        <v>43810</v>
+        <v>43804</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.45">
@@ -1465,9 +1435,7 @@
       <c r="D49" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E49" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="E49" s="1"/>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B50" s="5">
@@ -1479,64 +1447,58 @@
       <c r="D50" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E50" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="E50" s="1"/>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B51" s="5">
         <v>43810</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="C51" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E51" s="4"/>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B52" s="5">
         <v>43810</v>
       </c>
-      <c r="C52" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="C52" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E52" s="1"/>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B53" s="5">
         <v>43810</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>4</v>
+      <c r="C53" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B54" s="5">
         <v>43810</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>15</v>
+      <c r="C54" s="13" t="s">
+        <v>42</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.45">
@@ -1544,7 +1506,7 @@
         <v>43810</v>
       </c>
       <c r="C55" s="13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>7</v>
@@ -1558,13 +1520,13 @@
         <v>43810</v>
       </c>
       <c r="C56" s="13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.45">
@@ -1572,13 +1534,13 @@
         <v>43810</v>
       </c>
       <c r="C57" s="13" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.45">
@@ -1586,59 +1548,59 @@
         <v>43810</v>
       </c>
       <c r="C58" s="13" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>40</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E58" s="1"/>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B59" s="5">
         <v>43810</v>
       </c>
-      <c r="C59" s="13" t="s">
-        <v>45</v>
+      <c r="C59" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>40</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E59" s="1"/>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B60" s="5">
         <v>43810</v>
       </c>
-      <c r="C60" s="13" t="s">
-        <v>35</v>
+      <c r="C60" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E60" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B61" s="5">
         <v>43810</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E61" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B62" s="5">
         <v>43810</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>5</v>
@@ -1652,7 +1614,7 @@
         <v>43810</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>5</v>
@@ -1665,14 +1627,14 @@
       <c r="B64" s="5">
         <v>43810</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>50</v>
+      <c r="C64" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.45">
@@ -1680,234 +1642,466 @@
         <v>43810</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B66" s="5">
-        <v>43810</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>51</v>
+        <v>43811</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E66" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="E66" s="1"/>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B67" s="5">
-        <v>43810</v>
+        <v>43811</v>
       </c>
       <c r="C67" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E67" s="1"/>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B68" s="5">
+        <v>43811</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E68" s="4"/>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B69" s="5">
+        <v>43811</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E69" s="1"/>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B70" s="5">
+        <v>43811</v>
+      </c>
+      <c r="C70" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B71" s="5">
+        <v>43811</v>
+      </c>
+      <c r="C71" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B72" s="5">
+        <v>43811</v>
+      </c>
+      <c r="C72" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B73" s="5">
+        <v>43811</v>
+      </c>
+      <c r="C73" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B74" s="5">
+        <v>43811</v>
+      </c>
+      <c r="C74" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B75" s="5">
+        <v>43811</v>
+      </c>
+      <c r="C75" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E75" s="1"/>
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B76" s="5">
+        <v>43811</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E76" s="1"/>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B77" s="5">
+        <v>43811</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B78" s="5">
+        <v>43811</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B79" s="5">
+        <v>43811</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B80" s="5">
+        <v>43811</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B81" s="5">
+        <v>43811</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B82" s="5">
+        <v>43811</v>
+      </c>
+      <c r="C82" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D67" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E67" s="1" t="s">
+      <c r="D82" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E82" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B68" s="5"/>
-      <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
-    </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B69" s="5"/>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-    </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B70" s="5"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-    </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B71" s="5"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-    </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B72" s="5"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
-    </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B73" s="5"/>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
-    </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B74" s="5"/>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
-    </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B75" s="5"/>
-      <c r="C75" s="1"/>
-      <c r="D75" s="1"/>
-      <c r="E75" s="1"/>
-    </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B76" s="5"/>
-      <c r="C76" s="1"/>
-      <c r="D76" s="1"/>
-      <c r="E76" s="1"/>
-    </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B77" s="5"/>
-      <c r="C77" s="1"/>
-      <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
-    </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B78" s="5"/>
-      <c r="C78" s="1"/>
-      <c r="D78" s="1"/>
-      <c r="E78" s="1"/>
-    </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B79" s="5"/>
-      <c r="C79" s="1"/>
-      <c r="D79" s="1"/>
-      <c r="E79" s="1"/>
-    </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B80" s="5"/>
-      <c r="C80" s="1"/>
-      <c r="D80" s="1"/>
-      <c r="E80" s="1"/>
-    </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B81" s="5"/>
-      <c r="C81" s="1"/>
-      <c r="D81" s="1"/>
-      <c r="E81" s="1"/>
-    </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B82" s="5"/>
-      <c r="C82" s="1"/>
-      <c r="D82" s="1"/>
-      <c r="E82" s="1"/>
-    </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B83" s="5"/>
-      <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
+      <c r="B83" s="5">
+        <v>43812</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E83" s="1"/>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B84" s="5"/>
-      <c r="C84" s="1"/>
-      <c r="D84" s="1"/>
+      <c r="B84" s="5">
+        <v>43812</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E84" s="1"/>
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B85" s="5"/>
-      <c r="C85" s="1"/>
-      <c r="D85" s="1"/>
-      <c r="E85" s="1"/>
+      <c r="B85" s="5">
+        <v>43812</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E85" s="4"/>
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B86" s="5"/>
-      <c r="C86" s="1"/>
-      <c r="D86" s="1"/>
+      <c r="B86" s="5">
+        <v>43812</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E86" s="1"/>
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B87" s="5"/>
-      <c r="C87" s="1"/>
-      <c r="D87" s="1"/>
-      <c r="E87" s="1"/>
+      <c r="B87" s="5">
+        <v>43812</v>
+      </c>
+      <c r="C87" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B88" s="5"/>
-      <c r="C88" s="1"/>
-      <c r="D88" s="1"/>
-      <c r="E88" s="1"/>
+      <c r="B88" s="5">
+        <v>43812</v>
+      </c>
+      <c r="C88" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="89" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B89" s="5"/>
-      <c r="C89" s="1"/>
-      <c r="D89" s="1"/>
-      <c r="E89" s="1"/>
+      <c r="B89" s="5">
+        <v>43812</v>
+      </c>
+      <c r="C89" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B90" s="5"/>
-      <c r="C90" s="1"/>
-      <c r="D90" s="1"/>
-      <c r="E90" s="1"/>
+      <c r="B90" s="5">
+        <v>43812</v>
+      </c>
+      <c r="C90" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B91" s="5"/>
-      <c r="C91" s="1"/>
-      <c r="D91" s="1"/>
-      <c r="E91" s="1"/>
+      <c r="B91" s="5">
+        <v>43812</v>
+      </c>
+      <c r="C91" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B92" s="5"/>
-      <c r="C92" s="1"/>
-      <c r="D92" s="1"/>
+      <c r="B92" s="5">
+        <v>43812</v>
+      </c>
+      <c r="C92" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E92" s="1"/>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B93" s="5"/>
-      <c r="C93" s="1"/>
-      <c r="D93" s="1"/>
+      <c r="B93" s="5">
+        <v>43812</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E93" s="1"/>
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B94" s="5"/>
-      <c r="C94" s="1"/>
-      <c r="D94" s="1"/>
-      <c r="E94" s="1"/>
+      <c r="B94" s="5">
+        <v>43812</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B95" s="5"/>
-      <c r="C95" s="1"/>
-      <c r="D95" s="1"/>
-      <c r="E95" s="1"/>
+      <c r="B95" s="5">
+        <v>43812</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B96" s="5"/>
-      <c r="C96" s="1"/>
-      <c r="D96" s="1"/>
-      <c r="E96" s="1"/>
+      <c r="B96" s="5">
+        <v>43812</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B97" s="5"/>
-      <c r="C97" s="1"/>
-      <c r="D97" s="1"/>
-      <c r="E97" s="1"/>
+      <c r="B97" s="5">
+        <v>43812</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B98" s="5"/>
-      <c r="C98" s="1"/>
-      <c r="D98" s="1"/>
-      <c r="E98" s="1"/>
+      <c r="B98" s="5">
+        <v>43812</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="99" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B99" s="5"/>
-      <c r="C99" s="1"/>
-      <c r="D99" s="1"/>
-      <c r="E99" s="1"/>
+      <c r="B99" s="5">
+        <v>43812</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="100" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B100" s="5"/>
@@ -3223,61 +3417,33 @@
       <c r="D318" s="1"/>
       <c r="E318" s="1"/>
     </row>
-    <row r="319" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B319" s="5"/>
-      <c r="C319" s="1"/>
-      <c r="D319" s="1"/>
-      <c r="E319" s="1"/>
-    </row>
-    <row r="320" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B320" s="5"/>
-      <c r="C320" s="1"/>
-      <c r="D320" s="1"/>
-      <c r="E320" s="1"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="B31:B36 D31:E33 D34 B35:D36 E34:E36 C31:C34 B3:E30 C62:E64 D59:D60 D55:E58 B55:C60 B37:E54 B61:D61 E59:E64 D65:E65 B68:E118 C66:E67">
-    <cfRule type="expression" dxfId="9" priority="19">
+  <conditionalFormatting sqref="B32:B37 D32:E34 D35 B36:D37 E35:E37 C32:C35 B3:E31 D57:D58 D53:E56 B53:C58 B38:E52 B59:D59 E57:E62 B100:E116 D74:D75 D70:E73 E74:E82 B70:C75 B76:D82 B60:E69">
+    <cfRule type="expression" dxfId="5" priority="25">
       <formula>EXACT($D3, $G$4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="21">
+    <cfRule type="expression" dxfId="4" priority="27">
       <formula>EXACT($D3,$G$3)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C65">
-    <cfRule type="expression" dxfId="7" priority="7">
-      <formula>EXACT($D65, $G$4)</formula>
+  <conditionalFormatting sqref="D91:D92 D87:E90 E91:E99 C87:C92 C93:D99 B83:E83 C84:E86">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>EXACT($D83, $G$4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="8">
-      <formula>EXACT($D65,$G$3)</formula>
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>EXACT($D83,$G$3)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B62:B65">
-    <cfRule type="expression" dxfId="5" priority="5">
-      <formula>EXACT($D62, $G$4)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6">
-      <formula>EXACT($D62,$G$3)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B66">
-    <cfRule type="expression" dxfId="3" priority="3">
-      <formula>EXACT($D66, $G$4)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
-      <formula>EXACT($D66,$G$3)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B67">
+  <conditionalFormatting sqref="B84:B99">
     <cfRule type="expression" dxfId="1" priority="1">
-      <formula>EXACT($D67, $G$4)</formula>
+      <formula>EXACT($D84, $G$4)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="2">
-      <formula>EXACT($D67,$G$3)</formula>
+      <formula>EXACT($D84,$G$3)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D341" xr:uid="{610B11A9-AB2F-494B-BE3D-0A3BF9CE644D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D339" xr:uid="{610B11A9-AB2F-494B-BE3D-0A3BF9CE644D}">
       <formula1>$G$3:$G$4</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
comments, tests & metrics
</commit_message>
<xml_diff>
--- a/test_records.xlsx
+++ b/test_records.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-workspace\HackMe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E37F7B-07E5-4208-930A-83707B5E1F9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9EE5F5A-38F9-4C3C-9CE4-508FECC5D2D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10546" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10546" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Testing" sheetId="2" r:id="rId1"/>
+    <sheet name="Unit Tests" sheetId="2" r:id="rId1"/>
+    <sheet name="GUI Tests" sheetId="3" r:id="rId2"/>
+    <sheet name="Validation Tests" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="121">
   <si>
     <t>Date</t>
   </si>
@@ -241,12 +243,286 @@
   <si>
     <t>Test implemented correctly</t>
   </si>
+  <si>
+    <t>* MANUAL TESTS:</t>
+  </si>
+  <si>
+    <t>*  - test initialize - check wordOnClick is called when listViewWords is clicked</t>
+  </si>
+  <si>
+    <t>*  - test initialiseGame - check everything is initialised correctly</t>
+  </si>
+  <si>
+    <t>*  - test wordOnClick - tests: if word matches password, go to end; if word doesn't match,</t>
+  </si>
+  <si>
+    <t>*  check if num of letters in correct place is correct, and score is prevScore-250;</t>
+  </si>
+  <si>
+    <t>*  if incorrect and out of lives, then score is 0 and go to end screen</t>
+  </si>
+  <si>
+    <r>
+      <t>testNumberOfWords</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>()</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>testSizeOfWords</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>()</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>testGetPassword</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>()</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>testMatchPassword</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>()</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>testCorrectChars</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>()</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>testNextString</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>()</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>testMain</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>()</t>
+    </r>
+  </si>
+  <si>
+    <t>The game will display a series of words and symbols</t>
+  </si>
+  <si>
+    <t>all words will be of equal length</t>
+  </si>
+  <si>
+    <t>words will be clickable by the user to make a guess</t>
+  </si>
+  <si>
+    <t>250 points will be deducted for incorrect guesses</t>
+  </si>
+  <si>
+    <t>Aim of the game is to guess the correct word</t>
+  </si>
+  <si>
+    <t>each incorrect word guess will display the number of correct letters whose position is the same as in the correct word</t>
+  </si>
+  <si>
+    <t>1000 points awarded for a correct guess on the first try</t>
+  </si>
+  <si>
+    <t>allow the user to restart the game</t>
+  </si>
+  <si>
+    <t>have an option to exit the game</t>
+  </si>
+  <si>
+    <t>random non-alphanumeric symbols will also be displayed to separate the words</t>
+  </si>
+  <si>
+    <t>non-alphanumeric symbols will not be inserted into the middle of any words</t>
+  </si>
+  <si>
+    <t>The user loses if they take more than 4 attempts.</t>
+  </si>
+  <si>
+    <t>The score from the game-just-played will be printed to the screen</t>
+  </si>
+  <si>
+    <t>Once a correct word is found, a game over screen will display</t>
+  </si>
+  <si>
+    <t>Words will be removed once they have been confirmed as being an incorrect guess</t>
+  </si>
+  <si>
+    <t>The game will have a scoring system to add competitiveness</t>
+  </si>
+  <si>
+    <t>After selecting a word, the game will compare this guess the correct word and display how many letters are in the correct position.</t>
+  </si>
+  <si>
+    <t>The user wins if they select the correct word. </t>
+  </si>
+  <si>
+    <t>The user is taken to an end-screen after winning/losing.</t>
+  </si>
+  <si>
+    <t>On starting the game, a list of words is displayed (of the same length)</t>
+  </si>
+  <si>
+    <t>Functional Requirements</t>
+  </si>
+  <si>
+    <t>A ‘home screen’ will allow the user to open a high score leaderboard</t>
+  </si>
+  <si>
+    <t>A ‘home screen’ will allow the user to start playing the game</t>
+  </si>
+  <si>
+    <t>A ‘home screen’ will allow the user to open the options menu</t>
+  </si>
+  <si>
+    <t>Failed to implement due to time constraints. the internal functions were implemented, just not the UI, the UI controller methods and the display of the scoreboard.</t>
+  </si>
+  <si>
+    <t>Failed to implement due to time constraints. Was not deemed necessary for main game functionality.</t>
+  </si>
+  <si>
+    <t>The options menu will allow the user to change the game difficulty (longer words will provide a more difficult game experience</t>
+  </si>
+  <si>
+    <t>The options menu will allow the user to change game theme/colour</t>
+  </si>
+  <si>
+    <t>No option menu was implemented</t>
+  </si>
+  <si>
+    <t>Change difficulty was implemented in the 'home screen' instead, not in a options menu.</t>
+  </si>
+  <si>
+    <t>Non-Functional Requirements</t>
+  </si>
+  <si>
+    <t>Words will be stored externally in a .txt file</t>
+  </si>
+  <si>
+    <t>The game will support keyboard interaction</t>
+  </si>
+  <si>
+    <t>The score will start at 1000 points</t>
+  </si>
+  <si>
+    <t>250 points are deducted for each incorrect guess</t>
+  </si>
+  <si>
+    <t>The game selects a random word from those displayed as the password. </t>
+  </si>
+  <si>
+    <t>On each selection, the game compares the selection to the password, letter by letter.</t>
+  </si>
+  <si>
+    <t>A UI text element displays the selected word, and the number of matching characters. </t>
+  </si>
+  <si>
+    <t>A UI text element displays the number of remaining attempts</t>
+  </si>
+  <si>
+    <t>GUI Tests</t>
+  </si>
+  <si>
+    <t>Home Screen - Exit button exists the application</t>
+  </si>
+  <si>
+    <t>Home Screen - Easy button launches the Game Screen and Game Screen displays 'Easy-sized' words</t>
+  </si>
+  <si>
+    <t>Home Screen - Hard button launches the Game Screen and Game Screen displays 'Hard-sized' words</t>
+  </si>
+  <si>
+    <t>Home Screen - Medium button launches the Game Screen and Game Screen displays 'Medium-sized' words</t>
+  </si>
+  <si>
+    <t>Game Screen - Choosing intial incorrect word reduced no. of attempts to 3 &amp; displays correct number of matched chars</t>
+  </si>
+  <si>
+    <t>Game Screen - Choosing another incorrect word reduced no. of attempts to 2 &amp; displays correct number of matched chars</t>
+  </si>
+  <si>
+    <t>Game Screen - Choosing another incorrect word reduced no. of attempts to 1 &amp; displays correct number of matched chars</t>
+  </si>
+  <si>
+    <t>Game Screen - Choosing another incorrect word launches the end screen, with score of 0 displayed</t>
+  </si>
+  <si>
+    <t>Game Screen - Choosing correct word first time launches the end screen, with score of 1000</t>
+  </si>
+  <si>
+    <t>Game Screen - Choosing correct word the third time launches the end screen, with score of 500</t>
+  </si>
+  <si>
+    <t>Game Screen - Choosing correct word the second time launches the end screen, with score of 750</t>
+  </si>
+  <si>
+    <t>Game Screen - Choosing correct word the forth time launches the end screen, with score of 250</t>
+  </si>
+  <si>
+    <t>Game Screen - Choosing correct word second time launches the end screen, with score of 0</t>
+  </si>
+  <si>
+    <t>End Screen - Exit button exits the application</t>
+  </si>
+  <si>
+    <t>End Screen - Play again button launches the Home Screen</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -280,8 +556,22 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <i/>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF629755"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -303,6 +593,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2B2B2B"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -362,7 +658,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -377,11 +673,153 @@
     <xf numFmtId="14" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="26">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE84E18"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE84E18"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE84E18"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE84E18"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE84E18"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE84E18"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE84E18"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE84E18"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE84E18"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -724,8 +1162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5534E86-464A-458A-BDC4-36EF59462518}">
   <dimension ref="A1:G318"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="C100" sqref="C100"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2104,63 +2542,123 @@
       </c>
     </row>
     <row r="100" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B100" s="5"/>
-      <c r="C100" s="1"/>
-      <c r="D100" s="1"/>
+      <c r="B100" s="5">
+        <v>43816</v>
+      </c>
+      <c r="C100" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E100" s="1"/>
     </row>
     <row r="101" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B101" s="5"/>
-      <c r="C101" s="1"/>
-      <c r="D101" s="1"/>
+      <c r="B101" s="5">
+        <v>43816</v>
+      </c>
+      <c r="C101" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E101" s="1"/>
     </row>
     <row r="102" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B102" s="5"/>
-      <c r="C102" s="1"/>
-      <c r="D102" s="1"/>
+      <c r="B102" s="5">
+        <v>43816</v>
+      </c>
+      <c r="C102" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E102" s="1"/>
     </row>
     <row r="103" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B103" s="5"/>
-      <c r="C103" s="1"/>
-      <c r="D103" s="1"/>
+      <c r="B103" s="5">
+        <v>43816</v>
+      </c>
+      <c r="C103" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E103" s="1"/>
     </row>
     <row r="104" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B104" s="5"/>
-      <c r="C104" s="1"/>
-      <c r="D104" s="1"/>
+      <c r="B104" s="5">
+        <v>43816</v>
+      </c>
+      <c r="C104" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E104" s="1"/>
     </row>
     <row r="105" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B105" s="5"/>
-      <c r="C105" s="1"/>
-      <c r="D105" s="1"/>
+      <c r="B105" s="5">
+        <v>43816</v>
+      </c>
+      <c r="C105" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E105" s="1"/>
     </row>
     <row r="106" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B106" s="5"/>
-      <c r="C106" s="1"/>
-      <c r="D106" s="1"/>
+      <c r="B106" s="5">
+        <v>43816</v>
+      </c>
+      <c r="C106" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E106" s="1"/>
     </row>
     <row r="107" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B107" s="5"/>
-      <c r="C107" s="1"/>
-      <c r="D107" s="1"/>
+      <c r="B107" s="5">
+        <v>43816</v>
+      </c>
+      <c r="C107" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E107" s="1"/>
     </row>
     <row r="108" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B108" s="5"/>
-      <c r="C108" s="1"/>
-      <c r="D108" s="1"/>
+      <c r="B108" s="5">
+        <v>43816</v>
+      </c>
+      <c r="C108" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E108" s="1"/>
     </row>
     <row r="109" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B109" s="5"/>
-      <c r="C109" s="1"/>
-      <c r="D109" s="1"/>
+      <c r="B109" s="5">
+        <v>43816</v>
+      </c>
+      <c r="C109" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E109" s="1"/>
     </row>
     <row r="110" spans="2:5" x14ac:dyDescent="0.45">
@@ -3418,28 +3916,36 @@
       <c r="E318" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B32:B37 D32:E34 D35 B36:D37 E35:E37 C32:C35 B3:E31 D57:D58 D53:E56 B53:C58 B38:E52 B59:D59 E57:E62 B100:E116 D74:D75 D70:E73 E74:E82 B70:C75 B76:D82 B60:E69">
-    <cfRule type="expression" dxfId="5" priority="25">
+  <conditionalFormatting sqref="B32:B37 D32:E34 D35 B36:D37 E35:E37 C32:C35 B3:E31 D57:D58 D53:E56 B53:C58 B38:E52 B59:D59 E57:E62 D74:D75 D70:E73 E74:E82 B70:C75 B76:D82 B60:E69 B110:E116 B100:B109 D100:E109">
+    <cfRule type="expression" dxfId="19" priority="27">
       <formula>EXACT($D3, $G$4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="27">
+    <cfRule type="expression" dxfId="18" priority="29">
       <formula>EXACT($D3,$G$3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D91:D92 D87:E90 E91:E99 C87:C92 C93:D99 B83:E83 C84:E86">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="17" priority="5">
       <formula>EXACT($D83, $G$4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="16" priority="6">
       <formula>EXACT($D83,$G$3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B84:B99">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="15" priority="3">
       <formula>EXACT($D84, $G$4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="14" priority="4">
       <formula>EXACT($D84,$G$3)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C100:C109">
+    <cfRule type="expression" dxfId="13" priority="1">
+      <formula>EXACT($D100, $G$4)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="2">
+      <formula>EXACT($D100,$G$3)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -3450,4 +3956,641 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AEE26A3-225B-43D0-94CF-80249B7390A8}">
+  <dimension ref="A8:J23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="97.796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="8" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="J9" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="J10" s="15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="J11" s="15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="J12" s="15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="J13" s="15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A21" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A23" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="1" id="{74CCEA79-CE9A-4DF5-B0EC-28E3119BC684}">
+            <xm:f>EXACT($B9, 'Unit Tests'!$G$4)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFE84E18"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="expression" priority="2" id="{A75D34A3-4D59-43DA-A094-0E7B7A01791F}">
+            <xm:f>EXACT($B9,'Unit Tests'!$G$3)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF92D050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>A9:C23</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6170705F-3048-471B-8AD4-872A31A7BA82}">
+          <x14:formula1>
+            <xm:f>'Unit Tests'!$G$3:$G$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>B9:B23</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90201BCE-44B8-4074-875D-78597A6BE232}">
+  <dimension ref="A1:C36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="105.06640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A19" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A20" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A21" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A22" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A23" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A24" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A25" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A26" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="1"/>
+    </row>
+    <row r="28" spans="1:3" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A29" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A30" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="1"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A31" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A32" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="1"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A33" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A34" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A35" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="1"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A36" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B13:B26">
+    <cfRule type="expression" dxfId="11" priority="39">
+      <formula>EXACT($D15, $G$4)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="40">
+      <formula>EXACT($D15,$G$3)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="6" id="{90AFDE35-3E1C-44A2-BD58-1FF6C934E56B}">
+            <xm:f>EXACT($B2, 'Unit Tests'!$G$4)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFE84E18"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="expression" priority="7" id="{1BFB0CF7-ED73-4A57-8802-D2F1884AF15B}">
+            <xm:f>EXACT($B2,'Unit Tests'!$G$3)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF92D050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>A29:A36 C29:C36 A2:C28</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="1" id="{54DC4EEF-2060-4ADF-AC35-1D94D4124F48}">
+            <xm:f>EXACT($B29, 'Unit Tests'!$G$4)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFE84E18"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="expression" priority="2" id="{5BEC1A60-0F62-46DC-A7E5-2EF0DB5B365A}">
+            <xm:f>EXACT($B29,'Unit Tests'!$G$3)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF92D050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>B29:B36</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{29070232-20F6-420D-B8A3-F8495A4C2699}">
+          <x14:formula1>
+            <xm:f>'Unit Tests'!$G$3:$G$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B26 B29:B36</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>